<commit_message>
added 0719 riding for signatures
</commit_message>
<xml_diff>
--- a/DSSG2017_data/gas_station_data/official_CO_SO2.xlsx
+++ b/DSSG2017_data/gas_station_data/official_CO_SO2.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\01-Research\04 - Talat School\02-Calibration Data\JSTREET\JST Data (7-5 7-18)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myeong/git/Atl_DSSG/Cycle-Atlanta-SLaB/DSSG2017_data/gas_station_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,18 +30,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>SO2</t>
   </si>
   <si>
     <t>CO</t>
   </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>RH</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>NO2</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>PM25</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -348,26 +378,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>42928</v>
       </c>
@@ -380,8 +435,29 @@
       <c r="D2">
         <v>439.49308122907399</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>23.376549784342401</v>
+      </c>
+      <c r="F2">
+        <v>85.088336563110403</v>
+      </c>
+      <c r="G2">
+        <v>16.5008056958516</v>
+      </c>
+      <c r="H2">
+        <v>-2.7590521184417101E-3</v>
+      </c>
+      <c r="I2">
+        <v>5.7784818808237697</v>
+      </c>
+      <c r="J2">
+        <v>8.7827599287033102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>42928</v>
+      </c>
       <c r="B3">
         <v>1</v>
       </c>
@@ -391,8 +467,29 @@
       <c r="D3">
         <v>399.47030294166399</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>22.759580135345502</v>
+      </c>
+      <c r="F3">
+        <v>87.805537033081094</v>
+      </c>
+      <c r="G3">
+        <v>16.262961101531999</v>
+      </c>
+      <c r="H3">
+        <v>1.6450320000816001E-2</v>
+      </c>
+      <c r="I3">
+        <v>5.4046771764755297</v>
+      </c>
+      <c r="J3">
+        <v>8.1402271668116306</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>42928</v>
+      </c>
       <c r="B4">
         <v>2</v>
       </c>
@@ -402,8 +499,29 @@
       <c r="D4">
         <v>373.58593874561598</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>22.5712698936462</v>
+      </c>
+      <c r="F4">
+        <v>87.011013793945295</v>
+      </c>
+      <c r="G4">
+        <v>17.9091137568156</v>
+      </c>
+      <c r="H4">
+        <v>0.13122092085638201</v>
+      </c>
+      <c r="I4">
+        <v>5.73021121025086</v>
+      </c>
+      <c r="J4">
+        <v>8.6896309137344403</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>42928</v>
+      </c>
       <c r="B5">
         <v>3</v>
       </c>
@@ -413,8 +531,29 @@
       <c r="D5">
         <v>365.53924208421</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>22.4317545890808</v>
+      </c>
+      <c r="F5">
+        <v>86.095574188232405</v>
+      </c>
+      <c r="G5">
+        <v>12.706135336558001</v>
+      </c>
+      <c r="H5">
+        <v>2.57925587704807</v>
+      </c>
+      <c r="I5">
+        <v>12.385658828417499</v>
+      </c>
+      <c r="J5">
+        <v>9.8357082764307702</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>42928</v>
+      </c>
       <c r="B6">
         <v>4</v>
       </c>
@@ -424,8 +563,29 @@
       <c r="D6">
         <v>367.25837489536798</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>22.354143206278501</v>
+      </c>
+      <c r="F6">
+        <v>85.526397705078097</v>
+      </c>
+      <c r="G6">
+        <v>18.927009201049799</v>
+      </c>
+      <c r="H6">
+        <v>1.21378609812746</v>
+      </c>
+      <c r="I6">
+        <v>7.2893302957216903</v>
+      </c>
+      <c r="J6">
+        <v>8.9252619902292896</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>42928</v>
+      </c>
       <c r="B7">
         <v>5</v>
       </c>
@@ -435,8 +595,29 @@
       <c r="D7">
         <v>440.82007123839202</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>22.3839753786723</v>
+      </c>
+      <c r="F7">
+        <v>85.932991027832003</v>
+      </c>
+      <c r="G7">
+        <v>7.5976992686589497</v>
+      </c>
+      <c r="H7">
+        <v>8.5540709123015404</v>
+      </c>
+      <c r="I7">
+        <v>22.556744305292799</v>
+      </c>
+      <c r="J7">
+        <v>10.080099209149701</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>42928</v>
+      </c>
       <c r="B8">
         <v>6</v>
       </c>
@@ -446,8 +627,29 @@
       <c r="D8">
         <v>545.72420143594604</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>22.695969772338898</v>
+      </c>
+      <c r="F8">
+        <v>86.382223765055301</v>
+      </c>
+      <c r="G8">
+        <v>6.4291079759597798</v>
+      </c>
+      <c r="H8">
+        <v>9.2038349429766306</v>
+      </c>
+      <c r="I8">
+        <v>21.6774227619171</v>
+      </c>
+      <c r="J8">
+        <v>11.2360418796539</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>42928</v>
+      </c>
       <c r="B9">
         <v>7</v>
       </c>
@@ -457,8 +659,29 @@
       <c r="D9">
         <v>485.68651710366299</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>23.540939553578699</v>
+      </c>
+      <c r="F9">
+        <v>85.630096689859997</v>
+      </c>
+      <c r="G9">
+        <v>10.3477559089661</v>
+      </c>
+      <c r="H9">
+        <v>8.3665346304575596</v>
+      </c>
+      <c r="I9">
+        <v>18.4525737603505</v>
+      </c>
+      <c r="J9">
+        <v>10.1990439573924</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>42928</v>
+      </c>
       <c r="B10">
         <v>8</v>
       </c>
@@ -468,8 +691,29 @@
       <c r="D10">
         <v>439.91747922313499</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>24.637963549296099</v>
+      </c>
+      <c r="F10">
+        <v>83.959413401285801</v>
+      </c>
+      <c r="G10">
+        <v>18.158208386103301</v>
+      </c>
+      <c r="H10">
+        <v>3.2773814996083601</v>
+      </c>
+      <c r="I10">
+        <v>9.8532979091008492</v>
+      </c>
+      <c r="J10">
+        <v>10.099289409319599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>42928</v>
+      </c>
       <c r="B11">
         <v>9</v>
       </c>
@@ -479,8 +723,29 @@
       <c r="D11">
         <v>353.783431143131</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>26.446413866678899</v>
+      </c>
+      <c r="F11">
+        <v>78.048446400960302</v>
+      </c>
+      <c r="G11">
+        <v>31.748703066508</v>
+      </c>
+      <c r="H11">
+        <v>1.04657518664996</v>
+      </c>
+      <c r="I11">
+        <v>3.4774190505345701</v>
+      </c>
+      <c r="J11">
+        <v>9.6086081902186091</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>42928</v>
+      </c>
       <c r="B12">
         <v>10</v>
       </c>
@@ -490,8 +755,29 @@
       <c r="D12">
         <v>346.44999389648399</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>27.603887081146201</v>
+      </c>
+      <c r="F12">
+        <v>70.732175699869799</v>
+      </c>
+      <c r="G12">
+        <v>41.767945798238102</v>
+      </c>
+      <c r="H12">
+        <v>0.493069453040759</v>
+      </c>
+      <c r="I12">
+        <v>2.01906358798345</v>
+      </c>
+      <c r="J12">
+        <v>11.978834883372</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>42928</v>
+      </c>
       <c r="B13">
         <v>11</v>
       </c>
@@ -501,8 +787,29 @@
       <c r="D13">
         <v>340.77832952535402</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>28.6610690752665</v>
+      </c>
+      <c r="F13">
+        <v>61.9211366653442</v>
+      </c>
+      <c r="G13">
+        <v>47.118483988443998</v>
+      </c>
+      <c r="H13">
+        <v>0.28031961421171803</v>
+      </c>
+      <c r="I13">
+        <v>1.3546299755573299</v>
+      </c>
+      <c r="J13">
+        <v>10.5531485637029</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>42928</v>
+      </c>
       <c r="B14">
         <v>12</v>
       </c>
@@ -512,8 +819,29 @@
       <c r="D14">
         <v>337.60068434111901</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>29.547161197662401</v>
+      </c>
+      <c r="F14">
+        <v>58.021357282002803</v>
+      </c>
+      <c r="G14">
+        <v>45.661652692159002</v>
+      </c>
+      <c r="H14">
+        <v>0.20213748787840199</v>
+      </c>
+      <c r="I14">
+        <v>1.01339888374011</v>
+      </c>
+      <c r="J14">
+        <v>8.70174992084503</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>42928</v>
+      </c>
       <c r="B15">
         <v>13</v>
       </c>
@@ -523,8 +851,29 @@
       <c r="D15">
         <v>318.126204580631</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>30.331688117980999</v>
+      </c>
+      <c r="F15">
+        <v>52.826173845926903</v>
+      </c>
+      <c r="G15">
+        <v>43.843737157185899</v>
+      </c>
+      <c r="H15">
+        <v>0.30236852566401201</v>
+      </c>
+      <c r="I15">
+        <v>1.19541338781516</v>
+      </c>
+      <c r="J15">
+        <v>3.47384780182814</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>42928</v>
+      </c>
       <c r="B16">
         <v>14</v>
       </c>
@@ -534,8 +883,29 @@
       <c r="D16">
         <v>320.56875298947699</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>31.026372273762998</v>
+      </c>
+      <c r="F16">
+        <v>50.105187988281301</v>
+      </c>
+      <c r="G16">
+        <v>43.975451596577997</v>
+      </c>
+      <c r="H16">
+        <v>0.197633056156337</v>
+      </c>
+      <c r="I16">
+        <v>0.98508033355077096</v>
+      </c>
+      <c r="J16">
+        <v>1.7437185454803199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>42928</v>
+      </c>
       <c r="B17">
         <v>15</v>
       </c>
@@ -545,8 +915,29 @@
       <c r="D17">
         <v>330.56572737783802</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>31.3009671847026</v>
+      </c>
+      <c r="F17">
+        <v>51.1842041015625</v>
+      </c>
+      <c r="G17">
+        <v>49.794000116984101</v>
+      </c>
+      <c r="H17">
+        <v>0.20443918642898401</v>
+      </c>
+      <c r="I17">
+        <v>1.13688590625922</v>
+      </c>
+      <c r="J17">
+        <v>1.47627861946821</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>42928</v>
+      </c>
       <c r="B18">
         <v>16</v>
       </c>
@@ -556,8 +947,29 @@
       <c r="D18">
         <v>335.142832230549</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>31.546488030751501</v>
+      </c>
+      <c r="F18">
+        <v>50.49904200236</v>
+      </c>
+      <c r="G18">
+        <v>54.355473836263002</v>
+      </c>
+      <c r="H18">
+        <v>0.24277623593807199</v>
+      </c>
+      <c r="I18">
+        <v>1.57720871269703</v>
+      </c>
+      <c r="J18">
+        <v>6.5278675715128598</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>42928</v>
+      </c>
       <c r="B19">
         <v>17</v>
       </c>
@@ -567,8 +979,29 @@
       <c r="D19">
         <v>326.76281565540199</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>31.306494522094699</v>
+      </c>
+      <c r="F19">
+        <v>48.9425303777059</v>
+      </c>
+      <c r="G19">
+        <v>49.843865966796898</v>
+      </c>
+      <c r="H19">
+        <v>0.20151531087855501</v>
+      </c>
+      <c r="I19">
+        <v>1.50305213530858</v>
+      </c>
+      <c r="J19">
+        <v>5.2706647157669098</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>42928</v>
+      </c>
       <c r="B20">
         <v>18</v>
       </c>
@@ -578,8 +1011,29 @@
       <c r="D20">
         <v>335.23012994260199</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>30.626008828481002</v>
+      </c>
+      <c r="F20">
+        <v>52.1697843551636</v>
+      </c>
+      <c r="G20">
+        <v>42.613246409098302</v>
+      </c>
+      <c r="H20">
+        <v>0.14114107266068501</v>
+      </c>
+      <c r="I20">
+        <v>1.6841573933760301</v>
+      </c>
+      <c r="J20">
+        <v>6.6300709962844904</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>42928</v>
+      </c>
       <c r="B21">
         <v>19</v>
       </c>
@@ -589,8 +1043,29 @@
       <c r="D21">
         <v>344.81849756780701</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>29.2421869595846</v>
+      </c>
+      <c r="F21">
+        <v>64.887958272298206</v>
+      </c>
+      <c r="G21">
+        <v>32.571234830220497</v>
+      </c>
+      <c r="H21">
+        <v>2.56891568113739E-2</v>
+      </c>
+      <c r="I21">
+        <v>1.8320719738801301</v>
+      </c>
+      <c r="J21">
+        <v>13.4418979326884</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>42928</v>
+      </c>
       <c r="B22">
         <v>20</v>
       </c>
@@ -600,8 +1075,29 @@
       <c r="D22">
         <v>372.99045298050902</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>28.115174198150601</v>
+      </c>
+      <c r="F22">
+        <v>69.745408376057895</v>
+      </c>
+      <c r="G22">
+        <v>25.719341882069902</v>
+      </c>
+      <c r="H22">
+        <v>1.6312183035350099E-2</v>
+      </c>
+      <c r="I22">
+        <v>4.0848731623755601</v>
+      </c>
+      <c r="J22">
+        <v>7.9572635213533998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>42928</v>
+      </c>
       <c r="B23">
         <v>21</v>
       </c>
@@ -611,8 +1107,29 @@
       <c r="D23">
         <v>437.06670262263401</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>27.317402172088599</v>
+      </c>
+      <c r="F23">
+        <v>73.206538899739598</v>
+      </c>
+      <c r="G23">
+        <v>17.339873711268101</v>
+      </c>
+      <c r="H23">
+        <v>4.9035444793004798E-2</v>
+      </c>
+      <c r="I23">
+        <v>8.1499070876683994</v>
+      </c>
+      <c r="J23">
+        <v>6.4965191642443303</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>42928</v>
+      </c>
       <c r="B24">
         <v>22</v>
       </c>
@@ -622,8 +1139,29 @@
       <c r="D24">
         <v>458.20093200683601</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>26.469942792256699</v>
+      </c>
+      <c r="F24">
+        <v>73.327448145548502</v>
+      </c>
+      <c r="G24">
+        <v>15.965875449933501</v>
+      </c>
+      <c r="H24">
+        <v>1.07307360627601E-2</v>
+      </c>
+      <c r="I24">
+        <v>8.5309977610905996</v>
+      </c>
+      <c r="J24">
+        <v>7.7469554344812996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>42928</v>
+      </c>
       <c r="B25">
         <v>23</v>
       </c>
@@ -633,8 +1171,26 @@
       <c r="D25">
         <v>413.33937777005701</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>25.910601664397699</v>
+      </c>
+      <c r="F25">
+        <v>74.304588835118196</v>
+      </c>
+      <c r="G25">
+        <v>16.602517869737401</v>
+      </c>
+      <c r="H25">
+        <v>-1.3768227877608299E-2</v>
+      </c>
+      <c r="I25">
+        <v>7.7509670138359104</v>
+      </c>
+      <c r="J25">
+        <v>8.6407698534302799</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>42929</v>
       </c>
@@ -647,8 +1203,29 @@
       <c r="D26">
         <v>421.86804884307298</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>25.599008337656699</v>
+      </c>
+      <c r="F26">
+        <v>76.637965138753302</v>
+      </c>
+      <c r="G26">
+        <v>8.7577422102292406</v>
+      </c>
+      <c r="H26">
+        <v>2.74890357645151</v>
+      </c>
+      <c r="I26">
+        <v>13.9491782506307</v>
+      </c>
+      <c r="J26">
+        <v>7.7692181984583497</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>42929</v>
+      </c>
       <c r="B27">
         <v>1</v>
       </c>
@@ -658,8 +1235,29 @@
       <c r="D27">
         <v>419.21033066969699</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>25.1376730283101</v>
+      </c>
+      <c r="F27">
+        <v>80.024391682942706</v>
+      </c>
+      <c r="G27">
+        <v>4.0922880023717898</v>
+      </c>
+      <c r="H27">
+        <v>5.3629195970104799</v>
+      </c>
+      <c r="I27">
+        <v>18.0324374675751</v>
+      </c>
+      <c r="J27">
+        <v>7.2291962623596202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>42929</v>
+      </c>
       <c r="B28">
         <v>2</v>
       </c>
@@ -669,8 +1267,29 @@
       <c r="D28">
         <v>441.14160903619302</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>24.935211912790901</v>
+      </c>
+      <c r="F28">
+        <v>81.524099477132197</v>
+      </c>
+      <c r="G28">
+        <v>3.45879174868266</v>
+      </c>
+      <c r="H28">
+        <v>8.2966475476666002</v>
+      </c>
+      <c r="I28">
+        <v>19.684857789675402</v>
+      </c>
+      <c r="J28">
+        <v>7.5077327728271497</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>42929</v>
+      </c>
       <c r="B29">
         <v>3</v>
       </c>
@@ -680,8 +1299,29 @@
       <c r="D29">
         <v>458.28788639948903</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>24.613972377777099</v>
+      </c>
+      <c r="F29">
+        <v>81.946223576863602</v>
+      </c>
+      <c r="G29">
+        <v>5.5871169765790301</v>
+      </c>
+      <c r="H29">
+        <v>1.8486291827013099</v>
+      </c>
+      <c r="I29">
+        <v>11.9209254662196</v>
+      </c>
+      <c r="J29">
+        <v>7.4881573279698701</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>42929</v>
+      </c>
       <c r="B30">
         <v>4</v>
       </c>
@@ -691,8 +1331,29 @@
       <c r="D30">
         <v>469.55614300163398</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>24.484649753570601</v>
+      </c>
+      <c r="F30">
+        <v>81.307616043090803</v>
+      </c>
+      <c r="G30">
+        <v>0.84090995515386302</v>
+      </c>
+      <c r="H30">
+        <v>16.097488049666101</v>
+      </c>
+      <c r="I30">
+        <v>30.869137446085599</v>
+      </c>
+      <c r="J30">
+        <v>9.3226741313934305</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>42929</v>
+      </c>
       <c r="B31">
         <v>5</v>
       </c>
@@ -702,8 +1363,29 @@
       <c r="D31">
         <v>489.93316535230002</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>23.6924945831299</v>
+      </c>
+      <c r="F31">
+        <v>85.891856765747093</v>
+      </c>
+      <c r="G31">
+        <v>1.1589360762387499</v>
+      </c>
+      <c r="H31">
+        <v>8.6188581109046893</v>
+      </c>
+      <c r="I31">
+        <v>21.301493883132899</v>
+      </c>
+      <c r="J31">
+        <v>10.4009443124135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>42929</v>
+      </c>
       <c r="B32">
         <v>6</v>
       </c>
@@ -713,8 +1395,29 @@
       <c r="D32">
         <v>453.11095444036999</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>24.316249465942398</v>
+      </c>
+      <c r="F32">
+        <v>83.833437474568697</v>
+      </c>
+      <c r="G32">
+        <v>2.2166249476373201</v>
+      </c>
+      <c r="H32">
+        <v>19.9571678638458</v>
+      </c>
+      <c r="I32">
+        <v>31.789727528890001</v>
+      </c>
+      <c r="J32">
+        <v>10.439257899920101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>42929</v>
+      </c>
       <c r="B33">
         <v>7</v>
       </c>
@@ -724,8 +1427,29 @@
       <c r="D33">
         <v>467.41371183575302</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>26.0208653767904</v>
+      </c>
+      <c r="F33">
+        <v>77.438635762532599</v>
+      </c>
+      <c r="G33">
+        <v>8.9320526281992603</v>
+      </c>
+      <c r="H33">
+        <v>11.240809551874801</v>
+      </c>
+      <c r="I33">
+        <v>21.8068035125732</v>
+      </c>
+      <c r="J33">
+        <v>10.495019674301201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>42929</v>
+      </c>
       <c r="B34">
         <v>8</v>
       </c>
@@ -735,8 +1459,29 @@
       <c r="D34">
         <v>414.20992917430601</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>28.002996412912999</v>
+      </c>
+      <c r="F34">
+        <v>69.5391036987305</v>
+      </c>
+      <c r="G34">
+        <v>17.6364865779877</v>
+      </c>
+      <c r="H34">
+        <v>9.8444131056467707</v>
+      </c>
+      <c r="I34">
+        <v>20.623878637949598</v>
+      </c>
+      <c r="J34">
+        <v>13.4428657372793</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>42929</v>
+      </c>
       <c r="B35">
         <v>9</v>
       </c>
@@ -746,8 +1491,29 @@
       <c r="D35">
         <v>337.63997088738199</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>28.787621561686201</v>
+      </c>
+      <c r="F35">
+        <v>64.187203152974504</v>
+      </c>
+      <c r="G35">
+        <v>30.7229434013367</v>
+      </c>
+      <c r="H35">
+        <v>3.4001328294475899</v>
+      </c>
+      <c r="I35">
+        <v>8.8894555628299692</v>
+      </c>
+      <c r="J35">
+        <v>13.0481445789337</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>42929</v>
+      </c>
       <c r="B36">
         <v>10</v>
       </c>
@@ -757,8 +1523,29 @@
       <c r="D36">
         <v>338.56251121053901</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>29.751853370666499</v>
+      </c>
+      <c r="F36">
+        <v>57.451680183410602</v>
+      </c>
+      <c r="G36">
+        <v>48.412741661071799</v>
+      </c>
+      <c r="H36">
+        <v>0.52780385613441505</v>
+      </c>
+      <c r="I36">
+        <v>2.6490129709243799</v>
+      </c>
+      <c r="J36">
+        <v>10.912056016922</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>42929</v>
+      </c>
       <c r="B37">
         <v>11</v>
       </c>
@@ -768,8 +1555,29 @@
       <c r="D37">
         <v>349.88243131817501</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>30.514914925893098</v>
+      </c>
+      <c r="F37">
+        <v>54.853338050842297</v>
+      </c>
+      <c r="G37">
+        <v>58.495527712504099</v>
+      </c>
+      <c r="H37">
+        <v>0.27562712306777598</v>
+      </c>
+      <c r="I37">
+        <v>1.78752578298251</v>
+      </c>
+      <c r="J37">
+        <v>7.74084614912669</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>42929</v>
+      </c>
       <c r="B38">
         <v>12</v>
       </c>
@@ -779,8 +1587,29 @@
       <c r="D38">
         <v>362.61162644989599</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>31.198093636830599</v>
+      </c>
+      <c r="F38">
+        <v>53.211214764912903</v>
+      </c>
+      <c r="G38">
+        <v>63.447156715393099</v>
+      </c>
+      <c r="H38">
+        <v>0.41074010338634298</v>
+      </c>
+      <c r="I38">
+        <v>1.8894154449303899</v>
+      </c>
+      <c r="J38">
+        <v>5.7018196264902796</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>42929</v>
+      </c>
       <c r="B39">
         <v>13</v>
       </c>
@@ -790,8 +1619,29 @@
       <c r="D39">
         <v>383.227573610702</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>31.8857244173686</v>
+      </c>
+      <c r="F39">
+        <v>51.276168187459298</v>
+      </c>
+      <c r="G39">
+        <v>71.013195355733203</v>
+      </c>
+      <c r="H39">
+        <v>0.30709767105678698</v>
+      </c>
+      <c r="I39">
+        <v>2.0793767432371801</v>
+      </c>
+      <c r="J39">
+        <v>7.5910822769006101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>42929</v>
+      </c>
       <c r="B40">
         <v>14</v>
       </c>
@@ -801,8 +1651,29 @@
       <c r="D40">
         <v>376.52709524972101</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>31.885368982950801</v>
+      </c>
+      <c r="F40">
+        <v>50.864337221781398</v>
+      </c>
+      <c r="G40">
+        <v>73.690970611572297</v>
+      </c>
+      <c r="H40">
+        <v>0.42577907107770402</v>
+      </c>
+      <c r="I40">
+        <v>3.1260118226210301</v>
+      </c>
+      <c r="J40">
+        <v>7.5827110846837398</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>42929</v>
+      </c>
       <c r="B41">
         <v>15</v>
       </c>
@@ -812,8 +1683,29 @@
       <c r="D41">
         <v>397.56502892836102</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>31.771331914266</v>
+      </c>
+      <c r="F41">
+        <v>52.630072021484402</v>
+      </c>
+      <c r="G41">
+        <v>57.345469474792502</v>
+      </c>
+      <c r="H41">
+        <v>1.3277428209781701</v>
+      </c>
+      <c r="I41">
+        <v>7.3551390369733198</v>
+      </c>
+      <c r="J41">
+        <v>9.6049643993377707</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>42929</v>
+      </c>
       <c r="B42">
         <v>16</v>
       </c>
@@ -823,8 +1715,29 @@
       <c r="D42">
         <v>408.685723266602</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>29.307274182637499</v>
+      </c>
+      <c r="F42">
+        <v>64.840425046285006</v>
+      </c>
+      <c r="G42">
+        <v>44.599760723114002</v>
+      </c>
+      <c r="H42">
+        <v>0.43974628833432999</v>
+      </c>
+      <c r="I42">
+        <v>4.6572855432828302</v>
+      </c>
+      <c r="J42">
+        <v>10.965083018938699</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>42929</v>
+      </c>
       <c r="B43">
         <v>17</v>
       </c>
@@ -834,8 +1747,29 @@
       <c r="D43">
         <v>390.16460663417598</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>25.4160220464071</v>
+      </c>
+      <c r="F43">
+        <v>83.204108428955095</v>
+      </c>
+      <c r="G43">
+        <v>36.764801470438698</v>
+      </c>
+      <c r="H43">
+        <v>0.96265485205998003</v>
+      </c>
+      <c r="I43">
+        <v>6.1134895066420301</v>
+      </c>
+      <c r="J43">
+        <v>8.5550097485383301</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>42929</v>
+      </c>
       <c r="B44">
         <v>18</v>
       </c>
@@ -845,8 +1779,29 @@
       <c r="D44">
         <v>412.17912635024697</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>26.299822012583402</v>
+      </c>
+      <c r="F44">
+        <v>79.598268254597997</v>
+      </c>
+      <c r="G44">
+        <v>31.3117919286092</v>
+      </c>
+      <c r="H44">
+        <v>0.51567439362406697</v>
+      </c>
+      <c r="I44">
+        <v>7.0621899922688796</v>
+      </c>
+      <c r="J44">
+        <v>4.1011776937792703</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>42929</v>
+      </c>
       <c r="B45">
         <v>19</v>
       </c>
@@ -856,8 +1811,29 @@
       <c r="D45">
         <v>467.86671649285103</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>27.859023634592699</v>
+      </c>
+      <c r="F45">
+        <v>69.639314397176094</v>
+      </c>
+      <c r="G45">
+        <v>24.331820678710901</v>
+      </c>
+      <c r="H45">
+        <v>0.82787469162916205</v>
+      </c>
+      <c r="I45">
+        <v>11.267745939890499</v>
+      </c>
+      <c r="J45">
+        <v>7.6148500005404101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>42929</v>
+      </c>
       <c r="B46">
         <v>20</v>
       </c>
@@ -867,8 +1843,29 @@
       <c r="D46">
         <v>420.12888756576899</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>27.094856007893899</v>
+      </c>
+      <c r="F46">
+        <v>72.270092137654601</v>
+      </c>
+      <c r="G46">
+        <v>25.853539498647098</v>
+      </c>
+      <c r="H46">
+        <v>6.4561178847907297E-2</v>
+      </c>
+      <c r="I46">
+        <v>6.1295186042785703</v>
+      </c>
+      <c r="J46">
+        <v>10.370964646339401</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>42929</v>
+      </c>
       <c r="B47">
         <v>21</v>
       </c>
@@ -878,8 +1875,29 @@
       <c r="D47">
         <v>447.93087090386302</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>26.434068775177</v>
+      </c>
+      <c r="F47">
+        <v>78.094692103067999</v>
+      </c>
+      <c r="G47">
+        <v>9.5934184163808798</v>
+      </c>
+      <c r="H47">
+        <v>3.2051227405162899</v>
+      </c>
+      <c r="I47">
+        <v>18.000194215774499</v>
+      </c>
+      <c r="J47">
+        <v>10.965306878089899</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>42929</v>
+      </c>
       <c r="B48">
         <v>22</v>
       </c>
@@ -889,8 +1907,29 @@
       <c r="D48">
         <v>507.61506061164698</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>25.380731805165599</v>
+      </c>
+      <c r="F48">
+        <v>86.595978037516304</v>
+      </c>
+      <c r="G48">
+        <v>3.17230150417278</v>
+      </c>
+      <c r="H48">
+        <v>19.663703852954001</v>
+      </c>
+      <c r="I48">
+        <v>35.5715754191081</v>
+      </c>
+      <c r="J48">
+        <v>11.129293870925901</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>42929</v>
+      </c>
       <c r="B49">
         <v>23</v>
       </c>
@@ -900,8 +1939,26 @@
       <c r="D49">
         <v>605.47775926777001</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>25.388711315090401</v>
+      </c>
+      <c r="F49">
+        <v>86.558741682666906</v>
+      </c>
+      <c r="G49">
+        <v>1.5981920609871501</v>
+      </c>
+      <c r="H49">
+        <v>29.912561570183701</v>
+      </c>
+      <c r="I49">
+        <v>45.053064071526002</v>
+      </c>
+      <c r="J49">
+        <v>12.699961937079999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>42930</v>
       </c>
@@ -914,8 +1971,29 @@
       <c r="D50">
         <v>540.84638260821896</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>25.599826653798399</v>
+      </c>
+      <c r="F50">
+        <v>81.964874013265003</v>
+      </c>
+      <c r="G50">
+        <v>4.4488709350426996</v>
+      </c>
+      <c r="H50">
+        <v>4.8273874950905604</v>
+      </c>
+      <c r="I50">
+        <v>16.266827599207598</v>
+      </c>
+      <c r="J50">
+        <v>10.9666714509328</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>42930</v>
+      </c>
       <c r="B51">
         <v>1</v>
       </c>
@@ -925,8 +2003,29 @@
       <c r="D51">
         <v>461.70013024671999</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>25.018404483795202</v>
+      </c>
+      <c r="F51">
+        <v>85.142322031656903</v>
+      </c>
+      <c r="G51">
+        <v>5.7402869661649101</v>
+      </c>
+      <c r="H51">
+        <v>1.7106960808998899</v>
+      </c>
+      <c r="I51">
+        <v>10.290598471959401</v>
+      </c>
+      <c r="J51">
+        <v>10.6018022139867</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>42930</v>
+      </c>
       <c r="B52">
         <v>2</v>
       </c>
@@ -936,8 +2035,29 @@
       <c r="D52">
         <v>464.106820865553</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>24.157532787322999</v>
+      </c>
+      <c r="F52">
+        <v>90.372118631998703</v>
+      </c>
+      <c r="G52">
+        <v>2.8069957017898601</v>
+      </c>
+      <c r="H52">
+        <v>0.39254624682168199</v>
+      </c>
+      <c r="I52">
+        <v>8.9499100923538197</v>
+      </c>
+      <c r="J52">
+        <v>11.6596966266632</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>42930</v>
+      </c>
       <c r="B53">
         <v>3</v>
       </c>
@@ -947,8 +2067,29 @@
       <c r="D53">
         <v>437.19684952955998</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>23.956913757324202</v>
+      </c>
+      <c r="F53">
+        <v>90.090962600707996</v>
+      </c>
+      <c r="G53">
+        <v>3.3412866155306502</v>
+      </c>
+      <c r="H53">
+        <v>0.93269143551588096</v>
+      </c>
+      <c r="I53">
+        <v>8.8487299521764093</v>
+      </c>
+      <c r="J53">
+        <v>11.6466755390167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>42930</v>
+      </c>
       <c r="B54">
         <v>4</v>
       </c>
@@ -958,8 +2099,29 @@
       <c r="D54">
         <v>395.109816570671</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>23.738303120931</v>
+      </c>
+      <c r="F54">
+        <v>87.452714284261106</v>
+      </c>
+      <c r="G54">
+        <v>7.54142965475718</v>
+      </c>
+      <c r="H54">
+        <v>0.27654760634632097</v>
+      </c>
+      <c r="I54">
+        <v>6.53236514727275</v>
+      </c>
+      <c r="J54">
+        <v>11.661675675710001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>42930</v>
+      </c>
       <c r="B55">
         <v>5</v>
       </c>
@@ -969,8 +2131,29 @@
       <c r="D55">
         <v>383.69179031084201</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>23.460042381286598</v>
+      </c>
+      <c r="F55">
+        <v>87.554669062296597</v>
+      </c>
+      <c r="G55">
+        <v>8.3430585225423197</v>
+      </c>
+      <c r="H55">
+        <v>0.55409529029081295</v>
+      </c>
+      <c r="I55">
+        <v>6.5576145013173397</v>
+      </c>
+      <c r="J55">
+        <v>11.8005330721537</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>42930</v>
+      </c>
       <c r="B56">
         <v>6</v>
       </c>
@@ -980,8 +2163,29 @@
       <c r="D56">
         <v>395.916858906649</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>23.6452707608541</v>
+      </c>
+      <c r="F56">
+        <v>87.172152455647804</v>
+      </c>
+      <c r="G56">
+        <v>8.9971234083175702</v>
+      </c>
+      <c r="H56">
+        <v>1.88078769942125</v>
+      </c>
+      <c r="I56">
+        <v>7.0391795317332004</v>
+      </c>
+      <c r="J56">
+        <v>10.837352514267</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>42930</v>
+      </c>
       <c r="B57">
         <v>7</v>
       </c>
@@ -991,8 +2195,29 @@
       <c r="D57">
         <v>387.82681907797797</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>25.034998607635501</v>
+      </c>
+      <c r="F57">
+        <v>82.672677357991503</v>
+      </c>
+      <c r="G57">
+        <v>14.247938044865901</v>
+      </c>
+      <c r="H57">
+        <v>2.7573791662852001</v>
+      </c>
+      <c r="I57">
+        <v>6.8400963068008398</v>
+      </c>
+      <c r="J57">
+        <v>9.8466634353001901</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>42930</v>
+      </c>
       <c r="B58">
         <v>8</v>
       </c>
@@ -1002,8 +2227,29 @@
       <c r="D58">
         <v>581.75203002929698</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>26.9911305745443</v>
+      </c>
+      <c r="F58">
+        <v>76.079603068033904</v>
+      </c>
+      <c r="G58">
+        <v>23.712046496073398</v>
+      </c>
+      <c r="H58">
+        <v>1.8199852089087201</v>
+      </c>
+      <c r="I58">
+        <v>4.9621805270512898</v>
+      </c>
+      <c r="J58">
+        <v>11.690704965591401</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>42930</v>
+      </c>
       <c r="B59">
         <v>9</v>
       </c>
@@ -1013,8 +2259,29 @@
       <c r="D59">
         <v>366.57949771521203</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>28.7738405227661</v>
+      </c>
+      <c r="F59">
+        <v>68.448375320434593</v>
+      </c>
+      <c r="G59">
+        <v>35.030726814269997</v>
+      </c>
+      <c r="H59">
+        <v>1.58873221973578</v>
+      </c>
+      <c r="I59">
+        <v>4.1736556708812698</v>
+      </c>
+      <c r="J59">
+        <v>13.0596649328868</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>42930</v>
+      </c>
       <c r="B60">
         <v>10</v>
       </c>
@@ -1024,8 +2291,29 @@
       <c r="D60">
         <v>346.902785320671</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>30.186770121256501</v>
+      </c>
+      <c r="F60">
+        <v>59.710945765177399</v>
+      </c>
+      <c r="G60">
+        <v>39.905822118123403</v>
+      </c>
+      <c r="H60">
+        <v>0.33793871253728902</v>
+      </c>
+      <c r="I60">
+        <v>1.4495765482386</v>
+      </c>
+      <c r="J60">
+        <v>12.601932605107599</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>42930</v>
+      </c>
       <c r="B61">
         <v>11</v>
       </c>
@@ -1035,8 +2323,29 @@
       <c r="D61">
         <v>358.29739203819901</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>31.0578414916992</v>
+      </c>
+      <c r="F61">
+        <v>55.847871589660599</v>
+      </c>
+      <c r="G61">
+        <v>49.893633842468297</v>
+      </c>
+      <c r="H61">
+        <v>0.43817612528800998</v>
+      </c>
+      <c r="I61">
+        <v>2.19532862504323</v>
+      </c>
+      <c r="J61">
+        <v>11.2556918462117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>42930</v>
+      </c>
       <c r="B62">
         <v>12</v>
       </c>
@@ -1046,8 +2355,29 @@
       <c r="D62">
         <v>393.389220568599</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>31.380121199289999</v>
+      </c>
+      <c r="F62">
+        <v>54.402391560872402</v>
+      </c>
+      <c r="G62">
+        <v>60.4975325902303</v>
+      </c>
+      <c r="H62">
+        <v>1.0063304498791701</v>
+      </c>
+      <c r="I62">
+        <v>5.1563685377438899</v>
+      </c>
+      <c r="J62">
+        <v>11.329882756869001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>42930</v>
+      </c>
       <c r="B63">
         <v>13</v>
       </c>
@@ -1057,8 +2387,29 @@
       <c r="D63">
         <v>374.67495151735699</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>31.600926303863499</v>
+      </c>
+      <c r="F63">
+        <v>53.600498708089198</v>
+      </c>
+      <c r="G63">
+        <v>49.411634318033897</v>
+      </c>
+      <c r="H63">
+        <v>0.98505717317263297</v>
+      </c>
+      <c r="I63">
+        <v>4.3005172471205402</v>
+      </c>
+      <c r="J63">
+        <v>7.8894148548444099</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>42930</v>
+      </c>
       <c r="B64">
         <v>14</v>
       </c>
@@ -1068,8 +2419,29 @@
       <c r="D64">
         <v>370.661148382693</v>
       </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>32.178182697296101</v>
+      </c>
+      <c r="F64">
+        <v>51.9309986114502</v>
+      </c>
+      <c r="G64">
+        <v>41.002360661824603</v>
+      </c>
+      <c r="H64">
+        <v>1.6682654395699501</v>
+      </c>
+      <c r="I64">
+        <v>5.7480262994766198</v>
+      </c>
+      <c r="J64">
+        <v>6.9957361102104203</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>42930</v>
+      </c>
       <c r="B65">
         <v>15</v>
       </c>
@@ -1079,8 +2451,29 @@
       <c r="D65">
         <v>347.35971597524798</v>
       </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>32.485807609558101</v>
+      </c>
+      <c r="F65">
+        <v>49.592492039998398</v>
+      </c>
+      <c r="G65">
+        <v>41.648591105143197</v>
+      </c>
+      <c r="H65">
+        <v>0.44589522058765102</v>
+      </c>
+      <c r="I65">
+        <v>1.9977500100930501</v>
+      </c>
+      <c r="J65">
+        <v>4.5546512017647398</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>42930</v>
+      </c>
       <c r="B66">
         <v>16</v>
       </c>
@@ -1090,8 +2483,29 @@
       <c r="D66">
         <v>340.39349792480499</v>
       </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>32.404747645060198</v>
+      </c>
+      <c r="F66">
+        <v>47.608511288960798</v>
+      </c>
+      <c r="G66">
+        <v>40.137734476725299</v>
+      </c>
+      <c r="H66">
+        <v>0.247635756557186</v>
+      </c>
+      <c r="I66">
+        <v>1.3934805055459301</v>
+      </c>
+      <c r="J66">
+        <v>3.4868542949358599</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>42930</v>
+      </c>
       <c r="B67">
         <v>17</v>
       </c>
@@ -1101,8 +2515,29 @@
       <c r="D67">
         <v>336.416864934957</v>
       </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>31.753600470224999</v>
+      </c>
+      <c r="F67">
+        <v>52.267331441243499</v>
+      </c>
+      <c r="G67">
+        <v>35.272566668192503</v>
+      </c>
+      <c r="H67">
+        <v>0.28860023940602902</v>
+      </c>
+      <c r="I67">
+        <v>1.5903027534484899</v>
+      </c>
+      <c r="J67">
+        <v>2.10507196250061</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>42930</v>
+      </c>
       <c r="B68">
         <v>18</v>
       </c>
@@ -1112,8 +2547,29 @@
       <c r="D68">
         <v>346.35871357820503</v>
       </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>30.182104365030899</v>
+      </c>
+      <c r="F68">
+        <v>57.083882776896203</v>
+      </c>
+      <c r="G68">
+        <v>34.811544259389301</v>
+      </c>
+      <c r="H68">
+        <v>0.18350086901336901</v>
+      </c>
+      <c r="I68">
+        <v>1.9829413592815399</v>
+      </c>
+      <c r="J68">
+        <v>4.6620762204130504</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>42930</v>
+      </c>
       <c r="B69">
         <v>19</v>
       </c>
@@ -1123,8 +2579,29 @@
       <c r="D69">
         <v>335.17363926149801</v>
       </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>27.467173480987601</v>
+      </c>
+      <c r="F69">
+        <v>67.852468872070304</v>
+      </c>
+      <c r="G69">
+        <v>33.726555728912402</v>
+      </c>
+      <c r="H69">
+        <v>5.1091929342025298E-2</v>
+      </c>
+      <c r="I69">
+        <v>2.7851316610972101</v>
+      </c>
+      <c r="J69">
+        <v>9.6935807625452703</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>42930</v>
+      </c>
       <c r="B70">
         <v>20</v>
       </c>
@@ -1134,8 +2611,29 @@
       <c r="D70">
         <v>335.28599143514799</v>
       </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>26.182473341623901</v>
+      </c>
+      <c r="F70">
+        <v>69.095961252848298</v>
+      </c>
+      <c r="G70">
+        <v>34.962733936309803</v>
+      </c>
+      <c r="H70">
+        <v>1.7975575795086799E-3</v>
+      </c>
+      <c r="I70">
+        <v>2.5221881548563601</v>
+      </c>
+      <c r="J70">
+        <v>8.0475114504496208</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>42930</v>
+      </c>
       <c r="B71">
         <v>21</v>
       </c>
@@ -1145,8 +2643,29 @@
       <c r="D71">
         <v>368.19929993827401</v>
       </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>26.0971610069275</v>
+      </c>
+      <c r="F71">
+        <v>68.684592692057294</v>
+      </c>
+      <c r="G71">
+        <v>31.0457636197408</v>
+      </c>
+      <c r="H71">
+        <v>0.35597867937460098</v>
+      </c>
+      <c r="I71">
+        <v>7.3938544407868996</v>
+      </c>
+      <c r="J71">
+        <v>4.9305783453087004</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>42930</v>
+      </c>
       <c r="B72">
         <v>22</v>
       </c>
@@ -1156,8 +2675,29 @@
       <c r="D72">
         <v>388.25323361766601</v>
       </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>26.0662933031718</v>
+      </c>
+      <c r="F72">
+        <v>69.5671062469482</v>
+      </c>
+      <c r="G72">
+        <v>30.770398390920501</v>
+      </c>
+      <c r="H72">
+        <v>5.3393914674507E-2</v>
+      </c>
+      <c r="I72">
+        <v>5.4119245489438397</v>
+      </c>
+      <c r="J72">
+        <v>5.7139068702856699</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>42930</v>
+      </c>
       <c r="B73">
         <v>23</v>
       </c>
@@ -1166,6 +2706,24 @@
       </c>
       <c r="D73">
         <v>414.18790133494298</v>
+      </c>
+      <c r="E73">
+        <v>25.3116788546244</v>
+      </c>
+      <c r="F73">
+        <v>75.138305282592796</v>
+      </c>
+      <c r="G73">
+        <v>21.7104795301283</v>
+      </c>
+      <c r="H73">
+        <v>6.6423817798949604E-3</v>
+      </c>
+      <c r="I73">
+        <v>6.3500350626503499</v>
+      </c>
+      <c r="J73">
+        <v>5.48013672033946</v>
       </c>
     </row>
   </sheetData>

</xml_diff>